<commit_message>
mat, equ, veh - completo
</commit_message>
<xml_diff>
--- a/reportes/reportes_parte_diario.xlsx
+++ b/reportes/reportes_parte_diario.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Reporte Principal" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Materiales Usados" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Equipos Usados" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Vehículos Usados" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -418,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,22 +485,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ot5</t>
+          <t>wqrqr</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">ewtsdg w </t>
+          <t xml:space="preserve">sadfasf </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>wett</t>
+          <t>afafas</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>twetwet</t>
+          <t xml:space="preserve"> faf</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -514,17 +515,17 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>eyeyry</t>
+          <t>sadasd</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>eryy</t>
+          <t xml:space="preserve"> cccccc</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>gwryt</t>
+          <t>mmmmmmmm</t>
         </is>
       </c>
     </row>
@@ -534,22 +535,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>mnmn</t>
+          <t>fasfasf</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>nnmmn</t>
+          <t>afsasf</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>nmnhy</t>
+          <t>afssaf</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>fdhery</t>
+          <t>afasf</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -559,22 +560,22 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Sí</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>nin</t>
+          <t>qwrwqr</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>cfasf</t>
+          <t>safafsafs</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>cafraf</t>
+          <t>asfasf</t>
         </is>
       </c>
     </row>
@@ -584,22 +585,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>retye</t>
+          <t>qwrqr</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ggdfg</t>
+          <t>afdas</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>gdgw4</t>
+          <t>asfasf</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>eryery</t>
+          <t>afasf</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -614,217 +615,17 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>46436fsdsf</t>
+          <t>sffsa</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>fvcc c</t>
+          <t>ccccccccc</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>36246</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>45688</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>retye</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ggdfg</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>gdgw4</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>eryery</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>464yey36fsdsf</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>fvcc yy</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>36246yyy</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>45688</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>retye</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ggdfg</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>gdgw4</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>eryery</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>464yey36fsdsf</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>mmmmm</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>ccccccc</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>45688</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>hery</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>eyey</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>sgd</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>bbbb</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>ewtewt</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>dsgsdg</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>sdge4r4yer</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>45688</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>oi56</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>etwet twt</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>wete wq</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>wrrwrrw</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>mumyu</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>ytiuuty</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>ccccccc</t>
+          <t>mmmmmmmm</t>
         </is>
       </c>
     </row>
@@ -839,7 +640,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -930,17 +731,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ot5</t>
+          <t>wqrqr</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">ewtsdg w </t>
+          <t xml:space="preserve">sadfasf </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>BROCHA TUMI 2"</t>
+          <t>RODILLO TORO PELO BLANCO 1"</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -949,20 +750,46 @@
         </is>
       </c>
       <c r="F2" t="n">
+        <v>43</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>JET ZINC PRIMER 910 PARTE "B"</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>gln</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>THINER ACRILICO</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>gl</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>4</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>cemento andino</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>bolsa</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
         <v>5</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>DISCO DE CORTE CONCRETO  9"</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>und</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>65</v>
       </c>
     </row>
     <row r="3">
@@ -971,65 +798,26 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>mnmn</t>
+          <t>fasfasf</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>nnmmn</t>
+          <t>afsasf</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>BROCHA ECONOMICA 1"</t>
+          <t>gf</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>und</t>
+          <t>44r</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>mortero</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>und</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>7</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>DILUYENTE TRAFICO MAESTRO</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>gl</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>4</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>hola</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>bl</t>
-        </is>
-      </c>
-      <c r="O3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -1038,241 +826,51 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>retye</t>
+          <t>qwrqr</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ggdfg</t>
+          <t>afdas</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>DILUYENTE TRAFICO MAESTRO</t>
+          <t>PERNOS CABEZA DE COCHE 5/8" X 4" + TUERCA + ARANDELA</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>gl</t>
+          <t>und</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>PINTURA TRAFICO MAESTRO</t>
+          <t>cemento andino</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>gl</t>
+          <t>bs</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>cemento andino</t>
+          <t>LIJA AL AGUA #150</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>bolsa</t>
+          <t>und</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>45688</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>retye</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ggdfg</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>BROCHA ECONOMICA 2"</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>und</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>4</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>ARENA GRUESA</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>m3</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>45688</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>retye</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ggdfg</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>BROCHA ECONOMICA 2"</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>und</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>6</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>BROCHA TUMI 2"</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>und</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>66</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>RODILLO TORO PELO BLANCO 3"</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>und</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>45688</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>hery</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>eyey</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ARENA GRUESA</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>m3</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>6</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>SIKADUR 31 5KG</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>und</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>8</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>andino</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>bb</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>45688</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>oi56</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>etwet twt</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>BROCHA TUMI 2"</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>und</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>6</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>mjkmjm</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>ju</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1287,7 +885,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1378,12 +976,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ot5</t>
+          <t>wqrqr</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">ewtsdg w </t>
+          <t xml:space="preserve">sadfasf </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1392,10 +990,12 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>propio</t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -1403,10 +1003,25 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>5</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>propio</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>gata hidra</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>alquiladoo</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -1415,57 +1030,65 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>mnmn</t>
+          <t>fasfasf</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>nnmmn</t>
+          <t>afsasf</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Generador eléctrico de 20Kw</t>
+          <t>Reflectores LED</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>propio</t>
+        </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Amortiguador de impacto</t>
+          <t>ewr</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>3</v>
-      </c>
-      <c r="I3" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>rwrfdf</t>
+        </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Camión remolcador- amortiguador</t>
+          <t>Generador eléctrico de 7Kw</t>
         </is>
       </c>
       <c r="K3" t="n">
         <v>3</v>
       </c>
-      <c r="L3" t="b">
-        <v>1</v>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>propio</t>
+        </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>gata hidraulica</t>
+          <t>Generador eléctrico de 7Kw</t>
         </is>
       </c>
       <c r="N3" t="n">
-        <v>2</v>
-      </c>
-      <c r="O3" t="b">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>propio</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -1474,17 +1097,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>retye</t>
+          <t>qwrqr</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ggdfg</t>
+          <t>afdas</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Amortiguador de impacto</t>
+          <t>Generador eléctrico de 20Kw</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -1492,12 +1115,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Propio</t>
+          <t>propio</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Reflectores LED</t>
+          <t>Amoladoras de 9", 4 1/2" o 7"</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -1505,236 +1128,266 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Propio</t>
+          <t>propio</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>gata</t>
+          <t>Rodillo Bermero (chupetero)</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Alquilado</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+          <t>propio</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Código Obra</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Nombre Ingeniero</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Vehículo 1</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Placa 1</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Propiedad 1</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Vehículo 2</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Placa 2</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Propiedad 2</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Vehículo 3</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Placa 3</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Propiedad 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>45688</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>retye</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ggdfg</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Camión remolcador- amortiguador</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Propio</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Gata hiddd</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Alquilado</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>wqrqr</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sadfasf </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CAMIONETA</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>BJP-925</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>propio</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAMION MATERIAL </t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>BEL-824</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>propio</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>camioneta hilux</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>hhh-555</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>alquilaado</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>45688</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>retye</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ggdfg</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Amortiguador de impacto</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Propio</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Gata Hidraulica pr</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Propio</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>llave stilson</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>6</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Alquilado</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>fasfasf</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>afsasf</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CAMION ALQUILADO</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NNN-000</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>alquilado</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>dretewt</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>45ggrg</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>434gfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>45688</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>hery</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>eyey</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Amortiguador de impacto</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>4</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Propio</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Flecha luminosa a bateria y soporte</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>4</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Propio</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>llave stilson</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>4</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>porpio</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>gata hid</t>
-        </is>
-      </c>
-      <c r="N7" t="n">
-        <v>8</v>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>alkilado</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>45688</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>oi56</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>etwet twt</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Amortiguador de impacto</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>7</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Propio</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Flecha luminosa a bateria y soporte</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>4</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Propio</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>gata</t>
-        </is>
-      </c>
-      <c r="K8" t="n">
-        <v>5</v>
-      </c>
-      <c r="L8" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>qwrqr</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>afdas</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CAMION GRUA ALQUILADO</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>NNN-000</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>alquilado</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAMION MATERIAL </t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>BEL-824</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>propio</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>CAMIONETA</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>BJP-925</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>propio</t>
         </is>
       </c>
     </row>

</xml_diff>